<commit_message>
checked outputs for ngram for net and dbms
</commit_message>
<xml_diff>
--- a/output/dbms comparisio.xlsx
+++ b/output/dbms comparisio.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="211">
   <si>
     <t>Text</t>
   </si>
@@ -403,6 +403,255 @@
   </si>
   <si>
     <t>After preprocessing</t>
+  </si>
+  <si>
+    <t>['0.7', '0.59', '0.58']</t>
+  </si>
+  <si>
+    <t>['0.77', '0.73', '0.71']</t>
+  </si>
+  <si>
+    <t>['0.38', '0.38', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.49', '0.43', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.48', '0.46', '0.43']</t>
+  </si>
+  <si>
+    <t>['0.27', '0.26', '0.25']</t>
+  </si>
+  <si>
+    <t>['0.26', '0.25', '0.24']</t>
+  </si>
+  <si>
+    <t>['0.67', '0.37', '0.32']</t>
+  </si>
+  <si>
+    <t>['0.48', '0.44', '0.26']</t>
+  </si>
+  <si>
+    <t>['0.43', '0.43', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.75', '0.47', '0.43']</t>
+  </si>
+  <si>
+    <t>['0.43', '0.41', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.71', '0.4', '0.36']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.51', '0.5']</t>
+  </si>
+  <si>
+    <t>['0.49', '0.46', '0.46']</t>
+  </si>
+  <si>
+    <t>['0.74', '0.52', '0.51']</t>
+  </si>
+  <si>
+    <t>['0.33', '0.29', '0.26']</t>
+  </si>
+  <si>
+    <t>['0.5', '0.43', '0.4']</t>
+  </si>
+  <si>
+    <t>['0.48', '0.45', '0.41']</t>
+  </si>
+  <si>
+    <t>['0.94', '0.68', '0.65']</t>
+  </si>
+  <si>
+    <t>['0.46', '0.46', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.5', '0.37', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.76', '0.57', '0.55']</t>
+  </si>
+  <si>
+    <t>['0.58', '0.58', '0.56']</t>
+  </si>
+  <si>
+    <t>['0.48', '0.47', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.84', '0.67', '0.62']</t>
+  </si>
+  <si>
+    <t>['0.58', '0.57', '0.5']</t>
+  </si>
+  <si>
+    <t>['0.81', '0.74', '0.65']</t>
+  </si>
+  <si>
+    <t>['0.43', '0.34', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.49', '0.46', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.72', '0.46', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.7', '0.53', '0.48']</t>
+  </si>
+  <si>
+    <t>['0.44', '0.4', '0.34']</t>
+  </si>
+  <si>
+    <t>['0.84', '0.64', '0.6']</t>
+  </si>
+  <si>
+    <t>['0.5', '0.33', '0.3']</t>
+  </si>
+  <si>
+    <t>['0.36', '0.35', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.34', '0.28', '0.25']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.36', '0.32']</t>
+  </si>
+  <si>
+    <t>['0.36', '0.36', '0.34']</t>
+  </si>
+  <si>
+    <t>['0.43', '0.39', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.46', '0.45', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.55', '0.45', '0.42']</t>
+  </si>
+  <si>
+    <t>['0.67', '0.61', '0.56']</t>
+  </si>
+  <si>
+    <t>['0.51', '0.47', '0.46']</t>
+  </si>
+  <si>
+    <t>['0.53', '0.47', '0.44']</t>
+  </si>
+  <si>
+    <t>['0.36', '0.32', '0.31']</t>
+  </si>
+  <si>
+    <t>['0.22', '0.22', '0.21']</t>
+  </si>
+  <si>
+    <t>['0.66', '0.36', '0.35']</t>
+  </si>
+  <si>
+    <t>['0.5', '0.43', '0.24']</t>
+  </si>
+  <si>
+    <t>['0.48', '0.44', '0.39']</t>
+  </si>
+  <si>
+    <t>['0.69', '0.4', '0.38']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.55', '0.54']</t>
+  </si>
+  <si>
+    <t>['0.59', '0.56', '0.53']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.33', '0.28']</t>
+  </si>
+  <si>
+    <t>['0.54', '0.53', '0.5']</t>
+  </si>
+  <si>
+    <t>['0.68', '0.46', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.17', '0.16', '0.16']</t>
+  </si>
+  <si>
+    <t>['0.52', '0.41', '0.37']</t>
+  </si>
+  <si>
+    <t>['0.45', '0.45', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.82', '0.58', '0.57']</t>
+  </si>
+  <si>
+    <t>['0.45', '0.44', '0.43']</t>
+  </si>
+  <si>
+    <t>['0.61', '0.41', '0.4']</t>
+  </si>
+  <si>
+    <t>['0.73', '0.57', '0.5']</t>
+  </si>
+  <si>
+    <t>['0.44', '0.42', '0.41']</t>
+  </si>
+  <si>
+    <t>['0.55', '0.46', '0.46']</t>
+  </si>
+  <si>
+    <t>['0.83', '0.66', '0.65']</t>
+  </si>
+  <si>
+    <t>['0.62', '0.58', '0.55']</t>
+  </si>
+  <si>
+    <t>['0.7', '0.62', '0.57']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.39', '0.34']</t>
+  </si>
+  <si>
+    <t>['0.47', '0.45', '0.45']</t>
+  </si>
+  <si>
+    <t>['0.67', '0.45', '0.41']</t>
+  </si>
+  <si>
+    <t>['0.63', '0.46', '0.37']</t>
+  </si>
+  <si>
+    <t>['0.41', '0.37', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.7', '0.48', '0.47']</t>
+  </si>
+  <si>
+    <t>['0.5', '0.35', '0.34']</t>
+  </si>
+  <si>
+    <t>['0.29', '0.25', '0.24']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.33', '0.33']</t>
+  </si>
+  <si>
+    <t>['0.41', '0.39', '0.34']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.38', '0.32']</t>
+  </si>
+  <si>
+    <t>['0.44', '0.42', '0.42']</t>
+  </si>
+  <si>
+    <t>['0.4', '0.34', '0.33']</t>
+  </si>
+  <si>
+    <t>ngram(1,3) after prepro</t>
+  </si>
+  <si>
+    <t>ngram(1,3) without prepro</t>
   </si>
 </sst>
 </file>
@@ -1209,15 +1458,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="103.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1227,8 +1479,14 @@
       <c r="E1" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>209</v>
+      </c>
+      <c r="K1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1238,8 +1496,14 @@
       <c r="E2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1249,8 +1513,14 @@
       <c r="E3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>129</v>
+      </c>
+      <c r="K3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1260,8 +1530,14 @@
       <c r="E4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1271,8 +1547,14 @@
       <c r="E5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>131</v>
+      </c>
+      <c r="K5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1282,8 +1564,14 @@
       <c r="E6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1293,8 +1581,14 @@
       <c r="E7" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1304,8 +1598,14 @@
       <c r="E8" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -1315,8 +1615,14 @@
       <c r="E9" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>135</v>
+      </c>
+      <c r="K9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1326,8 +1632,14 @@
       <c r="E10" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>136</v>
+      </c>
+      <c r="K10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1337,8 +1649,14 @@
       <c r="E11" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1348,8 +1666,14 @@
       <c r="E12" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>138</v>
+      </c>
+      <c r="K12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1359,8 +1683,14 @@
       <c r="E13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1370,8 +1700,14 @@
       <c r="E14" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>139</v>
+      </c>
+      <c r="K14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1381,8 +1717,14 @@
       <c r="E15" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>140</v>
+      </c>
+      <c r="K15" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1392,8 +1734,14 @@
       <c r="E16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>141</v>
+      </c>
+      <c r="K16" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1403,8 +1751,14 @@
       <c r="E17" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>142</v>
+      </c>
+      <c r="K17" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1414,8 +1768,14 @@
       <c r="E18" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>143</v>
+      </c>
+      <c r="K18" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1425,8 +1785,14 @@
       <c r="E19" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>144</v>
+      </c>
+      <c r="K19" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1436,8 +1802,14 @@
       <c r="E20" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>145</v>
+      </c>
+      <c r="K20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1447,8 +1819,14 @@
       <c r="E21" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1458,8 +1836,14 @@
       <c r="E22" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>147</v>
+      </c>
+      <c r="K22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1469,8 +1853,14 @@
       <c r="E23" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>148</v>
+      </c>
+      <c r="K23" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1480,8 +1870,14 @@
       <c r="E24" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>149</v>
+      </c>
+      <c r="K24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1491,8 +1887,14 @@
       <c r="E25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>150</v>
+      </c>
+      <c r="K25" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1502,8 +1904,14 @@
       <c r="E26" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>151</v>
+      </c>
+      <c r="K26" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1513,8 +1921,14 @@
       <c r="E27" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>152</v>
+      </c>
+      <c r="K27" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1524,8 +1938,14 @@
       <c r="E28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>153</v>
+      </c>
+      <c r="K28" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1535,8 +1955,14 @@
       <c r="E29" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>154</v>
+      </c>
+      <c r="K29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1546,8 +1972,14 @@
       <c r="E30" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>155</v>
+      </c>
+      <c r="K30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1557,8 +1989,14 @@
       <c r="E31" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>156</v>
+      </c>
+      <c r="K31" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1568,8 +2006,14 @@
       <c r="E32" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>157</v>
+      </c>
+      <c r="K32" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1579,8 +2023,14 @@
       <c r="E33" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>158</v>
+      </c>
+      <c r="K33" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -1590,8 +2040,14 @@
       <c r="E34" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>159</v>
+      </c>
+      <c r="K34" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>68</v>
       </c>
@@ -1601,8 +2057,14 @@
       <c r="E35" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>160</v>
+      </c>
+      <c r="K35" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>70</v>
       </c>
@@ -1612,8 +2074,14 @@
       <c r="E36" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H36" t="s">
+        <v>161</v>
+      </c>
+      <c r="K36" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>72</v>
       </c>
@@ -1623,8 +2091,14 @@
       <c r="E37" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H37" t="s">
+        <v>162</v>
+      </c>
+      <c r="K37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -1634,8 +2108,14 @@
       <c r="E38" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H38" t="s">
+        <v>163</v>
+      </c>
+      <c r="K38" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>76</v>
       </c>
@@ -1645,8 +2125,14 @@
       <c r="E39" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H39" t="s">
+        <v>164</v>
+      </c>
+      <c r="K39" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>78</v>
       </c>
@@ -1656,8 +2142,14 @@
       <c r="E40" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H40" t="s">
+        <v>165</v>
+      </c>
+      <c r="K40" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1667,8 +2159,14 @@
       <c r="E41" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H41" t="s">
+        <v>166</v>
+      </c>
+      <c r="K41" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>82</v>
       </c>
@@ -1678,8 +2176,14 @@
       <c r="E42" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H42" t="s">
+        <v>167</v>
+      </c>
+      <c r="K42" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>84</v>
       </c>
@@ -1688,6 +2192,12 @@
       </c>
       <c r="E43" t="s">
         <v>126</v>
+      </c>
+      <c r="H43" t="s">
+        <v>168</v>
+      </c>
+      <c r="K43" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>